<commit_message>
Képváltó gombok hibájának javítása, az alkalmazás feltöltése kérdésekkel és a hozzájuk tartozó válaszokkal
- Korábbi hiba kezelve lett, az Ujjatek window két nyilas buttonjára
kattintva (mielőtt még kasztot választottunk volna) nem dob hibát az
alkalmazás.
- A kérdéseket tartalmazó fájl kiegészítve további kérdésekkel és
válaszokkal.
// Észlelt hiba: A Kerdesek window átalakításra szorul, mert a kérdést
tartalmazó TextBlocknak nincs sortörése, így egy hosszabb kérdés "kilóg"
a képernyőből, a végét nem lehet elolvasni. //
</commit_message>
<xml_diff>
--- a/Raetreon/bin/Debug/Fajlok/DB/kerdesadatbazis.xlsx
+++ b/Raetreon/bin/Debug/Fajlok/DB/kerdesadatbazis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Kérdés</t>
   </si>
@@ -23,18 +23,6 @@
     <t>Válasz</t>
   </si>
   <si>
-    <t>Hány feje van az embernek?</t>
-  </si>
-  <si>
-    <t>öt</t>
-  </si>
-  <si>
-    <t>Se oldala, se feneke, mégis megáll a víz benne.</t>
-  </si>
-  <si>
-    <t>felhő</t>
-  </si>
-  <si>
     <t>Édesanyád gyermeke, de neked nem testvéred, ki az?</t>
   </si>
   <si>
@@ -53,10 +41,124 @@
     <t>nevem</t>
   </si>
   <si>
-    <t>Aki nevemet kimondja, azonnal megsemmisít engem.</t>
-  </si>
-  <si>
-    <t>csend</t>
+    <t>Két szomszéd lakik egymás mellett, mindenkit látnak, csak egymást nem láthatják. Mi az?</t>
+  </si>
+  <si>
+    <t>Veled megyen, nincs teste, napsütésben fekete.</t>
+  </si>
+  <si>
+    <t>Fent lakom az égen, melegít a fényem, sugárból van bajszom, este van, ha alszom.</t>
+  </si>
+  <si>
+    <t>Szereted vagy nem szereted, ha megeszed, megkönnyezed.</t>
+  </si>
+  <si>
+    <t>A földben születik, nagy tűzben égetik, karikára nyújtják, az ujjadra húzzák.</t>
+  </si>
+  <si>
+    <t>Kis ember áll az erdőben, nagy kalap van a fejében. Ha kalapját megetted, őt magát is ismered.</t>
+  </si>
+  <si>
+    <t>Kint is van, bent is van, mégis csak a házban van.</t>
+  </si>
+  <si>
+    <t>Szekeremnek van kereke négy, de te azzal sehova se mégy. Én se ültem rajta soha még, messze van az ide, mint az ég.</t>
+  </si>
+  <si>
+    <t>Lába van, de mégse jár, víz felett visz, nem madár. Nem rab, mégis láncot hord, s minden utat összetold.</t>
+  </si>
+  <si>
+    <t>Kicsi is, görbe is. Tüzes még a feje is.</t>
+  </si>
+  <si>
+    <t>Erdőn voltam, parton leszek, vízen járok, s tűzben veszek. Mi az?</t>
+  </si>
+  <si>
+    <t>Kis koromban nyersen esznek, ízét adom a levesnek. Barátom a petrezselyem, egy csomóba kötik velem.</t>
+  </si>
+  <si>
+    <t>Zúgolódom, hangoskodom, pedig se szám, se pocakom, ami fogam alá kerül, megaprítom kegyetlenül, le azonban sosem nyelem, magam alá eresztgetem.</t>
+  </si>
+  <si>
+    <t>Egy doboz, nincs se pántja, kulcsa vagy fedele, de aranyló kincset rejt a belseje.</t>
+  </si>
+  <si>
+    <t>Mindent befal pofája, tátott szárnyast, szárnyatlant, fát, virágot, vasat csócsál, acélt ropogtat, fogával követ is kikoptat.</t>
+  </si>
+  <si>
+    <t>Él lélegzettelen, halotti hidegen, sose szomjas, kortya örök, páncélt hord, mi sose zörög.</t>
+  </si>
+  <si>
+    <t>Nem láthatni, nem tapinthatni, nem hallhatni, nem szagolhatni.Túl csillagokon, dombok tövében, kitölti az űrt egészen, sereghajtó, bár járt legelöl, életet végez, kacajt megöl.</t>
+  </si>
+  <si>
+    <t>Mi az, minek a gyökere lappang, a fáknál magasabb, fel, fel, fel az égre tör, és mégis sose nő?</t>
+  </si>
+  <si>
+    <t>30 fehér ló egy piros dombon, abrakolnak, dobrokolnak majd rajtuk a béklyó.</t>
+  </si>
+  <si>
+    <t>Hang nélkül kiált, szárnyatlan lebeg, fog nélkül kirág, szájatlan hebeg.</t>
+  </si>
+  <si>
+    <t>szem</t>
+  </si>
+  <si>
+    <t>árnyék</t>
+  </si>
+  <si>
+    <t>nap</t>
+  </si>
+  <si>
+    <t>hagyma</t>
+  </si>
+  <si>
+    <t>gyűrű</t>
+  </si>
+  <si>
+    <t>gomba</t>
+  </si>
+  <si>
+    <t>ablak</t>
+  </si>
+  <si>
+    <t>göncölszekér</t>
+  </si>
+  <si>
+    <t>híd</t>
+  </si>
+  <si>
+    <t>pipa</t>
+  </si>
+  <si>
+    <t>csónak</t>
+  </si>
+  <si>
+    <t>répa</t>
+  </si>
+  <si>
+    <t>fűrész</t>
+  </si>
+  <si>
+    <t>tojás</t>
+  </si>
+  <si>
+    <t>idő</t>
+  </si>
+  <si>
+    <t>hal</t>
+  </si>
+  <si>
+    <t>sötétség</t>
+  </si>
+  <si>
+    <t>hegy</t>
+  </si>
+  <si>
+    <t>fogak</t>
+  </si>
+  <si>
+    <t>szél</t>
   </si>
 </sst>
 </file>
@@ -389,15 +491,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="92.5703125" customWidth="1"/>
+    <col min="1" max="1" width="167.85546875" customWidth="1"/>
     <col min="2" max="2" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -408,32 +510,117 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -443,15 +630,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -461,32 +648,117 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>